<commit_message>
update to russian blanks
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/StockValidation.xlsx
+++ b/application/views/rpt/ru/StockValidation.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\isell3\application\views\rpt\ru\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="Акт звіряння" sheetId="1" r:id="rId1"/>
+    <sheet name="Остатки на складе" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
@@ -22,9 +27,6 @@
     <t>п/п</t>
   </si>
   <si>
-    <t>Залишок</t>
-  </si>
-  <si>
     <t>Склад</t>
   </si>
   <si>
@@ -52,13 +54,16 @@
     <t>Название</t>
   </si>
   <si>
-    <t>Перевірив_______________________________</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Виписав________________________________ /{$v-&gt;user_sign}/  </t>
-  </si>
-  <si>
-    <t>Залишки на складі ({$v-&gt;cat_name}) на {$v-&gt;date}</t>
+    <t>Остатки на складе ({$v-&gt;cat_name}) на {$v-&gt;date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Виписал________________________________ /{$v-&gt;user_sign}/  </t>
+  </si>
+  <si>
+    <t>Проверил_______________________________</t>
+  </si>
+  <si>
+    <t>Остаток</t>
   </si>
 </sst>
 </file>
@@ -334,27 +339,6 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -375,6 +359,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +452,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,7 +487,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +699,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,110 +707,110 @@
     <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="64.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14" style="17" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="A1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="22"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="16"/>
+      <c r="B3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="22" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>10</v>
       </c>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>